<commit_message>
This file contains all the URLs/APIs
</commit_message>
<xml_diff>
--- a/Ekart.xlsx
+++ b/Ekart.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\Ekart Spring Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC40347-C8CE-4A84-A568-699F5D431610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23008C52-1B35-4887-ACBC-5D0CD139CC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{D2D98E18-4518-4405-8968-160DFD6E8EB3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="88">
   <si>
     <t>Seller</t>
   </si>
@@ -287,6 +287,21 @@
   </si>
   <si>
     <t>Search all sellers of a product with given product Id</t>
+  </si>
+  <si>
+    <t>/buyers/deals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get the deals </t>
+  </si>
+  <si>
+    <t>Update product name, price, discount</t>
+  </si>
+  <si>
+    <t>/random/{category}</t>
+  </si>
+  <si>
+    <t>Get random product from a specific category</t>
   </si>
 </sst>
 </file>
@@ -370,12 +385,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -390,10 +402,19 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1067,95 +1088,95 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="K3" s="6" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="K3" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="K6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="3" t="s">
+      <c r="K8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="K11" s="6" t="s">
+      <c r="K11" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="K12" s="7" t="s">
+      <c r="K12" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="K13" s="3" t="s">
+      <c r="K13" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="K14" s="3" t="s">
+      <c r="K14" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="K15" s="3" t="s">
+      <c r="K15" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="K16" s="8" t="s">
+      <c r="K16" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K17" s="3" t="s">
+      <c r="K17" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="11:11" x14ac:dyDescent="0.3">
-      <c r="K18" s="7" t="s">
+      <c r="K18" s="6" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1167,296 +1188,339 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C09EF4-EDAA-4C84-B4F8-DEDC633386DF}">
-  <dimension ref="B2:K12"/>
+  <dimension ref="B2:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="44" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" style="1" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="45.33203125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="H2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="I2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="J2" s="9" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="1">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B3" s="10">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="1">
+      <c r="G3" s="10">
         <v>1</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="H3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J3" t="s">
+      <c r="I3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K3" t="s">
+      <c r="J3" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="1">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B4" s="10">
         <v>2</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="1">
+      <c r="G4" s="10">
         <v>2</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="H4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J4" t="s">
+      <c r="I4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K4" t="s">
+      <c r="J4" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="1">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5" s="10">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="1">
+      <c r="G5" s="10">
         <v>3</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="H5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J5" t="s">
+      <c r="I5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K5" t="s">
+      <c r="J5" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="1">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="10">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="1">
+      <c r="G6" s="10">
         <v>4</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="H6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J6" t="s">
+      <c r="I6" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="K6" t="s">
+      <c r="J6" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="1">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7" s="10">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="1">
+      <c r="G7" s="10">
         <v>5</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="H7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J7" t="s">
+      <c r="I7" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K7" t="s">
+      <c r="J7" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="1">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8" s="10">
         <v>6</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="1">
+      <c r="G8" s="10">
         <v>6</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="H8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J8" t="s">
+      <c r="I8" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="K8" t="s">
+      <c r="J8" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="1">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="10">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="1">
+      <c r="G9" s="10">
         <v>7</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="H9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J9" t="s">
+      <c r="I9" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="K9" t="s">
+      <c r="J9" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10" s="10">
         <v>8</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="1">
+      <c r="G10" s="10">
         <v>8</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="H10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J10" t="s">
+      <c r="I10" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="K10" t="s">
+      <c r="J10" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="1">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="10">
         <v>9</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="1">
+      <c r="G11" s="10">
         <v>9</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="H11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J11" t="s">
+      <c r="I11" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="K11" t="s">
+      <c r="J11" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="H12" s="1">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G12" s="10">
         <v>10</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="H12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J12" t="s">
+      <c r="I12" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="K12" t="s">
+      <c r="J12" s="2" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G13" s="10">
+        <v>11</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G14" s="10">
+        <v>12</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G15" s="11">
+        <v>13</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1469,185 +1533,185 @@
   <dimension ref="C3:Q10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:G10"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.77734375" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.77734375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="4" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="N4" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="O4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="P4" s="10" t="s">
+      <c r="P4" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="Q4" s="10" t="s">
+      <c r="Q4" s="8" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <v>1</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <v>1</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="3">
         <v>12000</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5" s="3">
         <v>10</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="Q5" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="3">
         <v>2</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="3">
         <v>1</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="M6" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="3">
         <v>23000</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="3">
         <v>15</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="P6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="Q6" s="4" t="s">
+      <c r="Q6" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <v>3</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="3">
         <v>2</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="3">
         <v>2000</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="3">
         <v>5</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="P7" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="Q7" s="4" t="s">
+      <c r="Q7" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="8" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="3">
         <v>4</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="3">
         <v>2</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8" s="3">
         <v>15000</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O8" s="3">
         <v>12</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="P8" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="Q8" s="4" t="s">
+      <c r="Q8" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="9" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="10" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>